<commit_message>
Limpeza dos dados em Python e no Power BI
</commit_message>
<xml_diff>
--- a/ETL/Filosofos.xlsx
+++ b/ETL/Filosofos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.silveira\Desktop\Pessoal\WebScraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.silveira\Desktop\Pessoal\WebScraping-Filosofos-Grecia\ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$358</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -480,7 +483,7 @@
     <t>Cálicles</t>
   </si>
   <si>
-    <t>Sofística?</t>
+    <t xml:space="preserve">Sofística </t>
   </si>
   <si>
     <t>Califonte</t>
@@ -687,7 +690,7 @@
     <t>Demócrates</t>
   </si>
   <si>
-    <t>Pitagórica?</t>
+    <t xml:space="preserve">Pitagórica </t>
   </si>
   <si>
     <t>Demócrito</t>
@@ -2019,7 +2022,7 @@
   <dimension ref="A1:D358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5513,6 +5516,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D358"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>